<commit_message>
Adding normal_values and fixing 34_ms_nance
</commit_message>
<xml_diff>
--- a/34_ms_nance/ms_nance_data.xlsx
+++ b/34_ms_nance/ms_nance_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="93">
   <si>
     <t>Variable</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>***Ms. Nance would not stand up for exercise</t>
   </si>
   <si>
     <t>Cardiac Output</t>
@@ -790,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:D97"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -802,7 +799,7 @@
     <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45.75" thickBot="1">
+    <row r="2" spans="1:4" ht="30.75" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -830,7 +827,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30.75" thickBot="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -844,7 +841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30.75" thickBot="1">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -858,7 +855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45.75" thickBot="1">
+    <row r="5" spans="1:4" ht="30.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1319,26 +1316,24 @@
       <c r="B38" s="4">
         <v>69</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>48</v>
+      <c r="C38" s="4">
+        <v>125</v>
+      </c>
+      <c r="D38" s="4">
+        <v>135</v>
+      </c>
+      <c r="E38" s="4">
+        <v>149</v>
+      </c>
+      <c r="F38" s="4">
+        <v>149</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60">
-      <c r="A39" s="6" t="s">
-        <v>49</v>
-      </c>
+    <row r="39" spans="1:7">
+      <c r="A39" s="6"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="41" spans="1:7" ht="16.5" thickBot="1">
@@ -1357,7 +1352,7 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1">
       <c r="A42" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" s="4">
         <v>3965</v>
@@ -1366,12 +1361,12 @@
         <v>5360</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1">
       <c r="A43" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="4">
         <v>57</v>
@@ -1380,7 +1375,7 @@
         <v>73</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1">
@@ -1394,7 +1389,7 @@
         <v>73</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1"/>
@@ -1414,7 +1409,7 @@
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1">
       <c r="A47" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B47" s="4">
         <v>65</v>
@@ -1428,7 +1423,7 @@
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1">
       <c r="A48" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" s="4">
         <v>8.1</v>
@@ -1442,7 +1437,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1">
       <c r="A49" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" s="4">
         <v>8.6999999999999993</v>
@@ -1456,7 +1451,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50" s="4">
         <v>3.6</v>
@@ -1470,7 +1465,7 @@
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1">
       <c r="A51" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" s="4">
         <v>27</v>
@@ -1484,7 +1479,7 @@
     </row>
     <row r="52" spans="1:4" ht="15.75" thickBot="1">
       <c r="A52" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" s="4">
         <v>26</v>
@@ -1498,7 +1493,7 @@
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1">
       <c r="A53" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53" s="4">
         <v>25.6</v>
@@ -1512,7 +1507,7 @@
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1">
       <c r="A54" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54" s="4">
         <v>24.4</v>
@@ -1541,7 +1536,7 @@
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1">
       <c r="A57" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="4">
         <v>24.3</v>
@@ -1555,7 +1550,7 @@
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1">
       <c r="A58" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" s="4">
         <v>144</v>
@@ -1564,12 +1559,12 @@
         <v>121</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1">
       <c r="A59" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" s="4">
         <v>87</v>
@@ -1583,7 +1578,7 @@
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1">
       <c r="A60" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" s="4">
         <v>87</v>
@@ -1592,12 +1587,12 @@
         <v>48</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1">
       <c r="A61" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B61" s="4">
         <v>57</v>
@@ -1606,12 +1601,12 @@
         <v>73</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30.75" thickBot="1">
       <c r="A62" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" s="4">
         <v>40</v>
@@ -1640,7 +1635,7 @@
     </row>
     <row r="65" spans="1:4" ht="15.75" thickBot="1">
       <c r="A65" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65" s="4">
         <v>6.0000000000000001E-3</v>
@@ -1649,12 +1644,12 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" thickBot="1">
       <c r="A66" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
@@ -1663,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1"/>
@@ -1683,7 +1678,7 @@
     </row>
     <row r="69" spans="1:4" ht="15.75" thickBot="1">
       <c r="A69" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69" s="4">
         <v>118</v>
@@ -1692,12 +1687,12 @@
         <v>180</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" thickBot="1">
       <c r="A70" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70" s="4">
         <v>62</v>
@@ -1706,7 +1701,7 @@
         <v>129</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" thickBot="1">
@@ -1725,7 +1720,7 @@
     </row>
     <row r="72" spans="1:4" ht="15.75" thickBot="1">
       <c r="A72" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" s="4">
         <v>2.1</v>
@@ -1739,7 +1734,7 @@
     </row>
     <row r="74" spans="1:4" ht="15.75">
       <c r="A74" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" thickBot="1"/>
@@ -1759,7 +1754,7 @@
     </row>
     <row r="77" spans="1:4" ht="15.75" thickBot="1">
       <c r="A77" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="4">
         <v>180</v>
@@ -1768,12 +1763,12 @@
         <v>180</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" thickBot="1">
       <c r="A78" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78" s="4">
         <v>87.84</v>
@@ -1782,7 +1777,7 @@
         <v>180</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1"/>
@@ -1802,7 +1797,7 @@
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1">
       <c r="A81" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" s="4">
         <v>5823</v>
@@ -1811,12 +1806,12 @@
         <v>5400</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75" thickBot="1">
       <c r="A82" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="4">
         <v>2303</v>
@@ -1825,12 +1820,12 @@
         <v>2400</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="30.75" thickBot="1">
       <c r="A83" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" s="4">
         <v>3520</v>
@@ -1839,7 +1834,7 @@
         <v>3000</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.75" thickBot="1"/>
@@ -1859,7 +1854,7 @@
     </row>
     <row r="86" spans="1:4" ht="30.75" thickBot="1">
       <c r="A86" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B86" s="4">
         <v>50.1</v>
@@ -1868,12 +1863,12 @@
         <v>43.2</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.75" thickBot="1">
       <c r="A87" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" s="4">
         <v>21.1</v>
@@ -1882,12 +1877,12 @@
         <v>15</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.75" thickBot="1">
       <c r="A88" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" s="4">
         <v>3.5</v>
@@ -1896,12 +1891,12 @@
         <v>3</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75" thickBot="1">
       <c r="A89" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" s="4">
         <v>17.5</v>
@@ -1910,12 +1905,12 @@
         <v>12</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" thickBot="1">
       <c r="A90" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" s="4">
         <v>0.1</v>
@@ -1924,12 +1919,12 @@
         <v>0</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1">
       <c r="A91" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" s="4">
         <v>0</v>
@@ -1938,12 +1933,12 @@
         <v>0</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" thickBot="1">
       <c r="A92" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" s="4">
         <v>29</v>
@@ -1952,7 +1947,7 @@
         <v>28.2</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" thickBot="1"/>
@@ -1972,7 +1967,7 @@
     </row>
     <row r="95" spans="1:4" ht="30.75" thickBot="1">
       <c r="A95" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B95" s="4">
         <v>26</v>
@@ -1986,7 +1981,7 @@
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1">
       <c r="A96" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" s="4">
         <v>26</v>
@@ -2000,7 +1995,7 @@
     </row>
     <row r="97" spans="1:4" ht="15.75" thickBot="1">
       <c r="A97" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B97" s="4">
         <v>0</v>
@@ -2009,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making changes to Lab 34
</commit_message>
<xml_diff>
--- a/34_ms_nance/ms_nance_data.xlsx
+++ b/34_ms_nance/ms_nance_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="106">
   <si>
     <t>Variable</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Venous Blood Gases</t>
-  </si>
-  <si>
-    <t>Arterial blood Gases</t>
   </si>
   <si>
     <t>Time</t>
@@ -335,6 +332,48 @@
   </si>
   <si>
     <t>Filtration</t>
+  </si>
+  <si>
+    <t>Initial chart</t>
+  </si>
+  <si>
+    <t>Initial Venous Blood</t>
+  </si>
+  <si>
+    <t>Arterial Blood Gases</t>
+  </si>
+  <si>
+    <t>Exercise tolerance, initial</t>
+  </si>
+  <si>
+    <t>Initial Cardiac Flow</t>
+  </si>
+  <si>
+    <t>Initial blood pressures</t>
+  </si>
+  <si>
+    <t>Left heart pressure and volume, initial</t>
+  </si>
+  <si>
+    <t>Left heart contractility, initial</t>
+  </si>
+  <si>
+    <t>Left heart blood flow, initial</t>
+  </si>
+  <si>
+    <t>Dietary, initial</t>
+  </si>
+  <si>
+    <t>Urinary, initial</t>
+  </si>
+  <si>
+    <t>Blood volume, initial</t>
+  </si>
+  <si>
+    <t>Water, initial</t>
+  </si>
+  <si>
+    <t>Lung fluids, initial</t>
   </si>
 </sst>
 </file>
@@ -785,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -799,7 +838,7 @@
     <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30.75" thickBot="1">
+    <row r="2" spans="1:5" ht="30.75" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -826,8 +865,11 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -841,7 +883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -855,7 +897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30.75" thickBot="1">
+    <row r="5" spans="1:5" ht="30.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -869,8 +911,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -897,8 +939,11 @@
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -912,7 +957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -926,7 +971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -940,7 +985,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -954,7 +999,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -968,7 +1013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -982,12 +1027,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A15" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16.5" thickBot="1">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
@@ -1014,8 +1057,11 @@
       <c r="D17" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -1029,7 +1075,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
@@ -1043,7 +1089,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
@@ -1057,7 +1103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1071,7 +1117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
@@ -1085,7 +1131,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1">
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
@@ -1099,12 +1145,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A24" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="16.5" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
@@ -1131,8 +1175,11 @@
       <c r="D26" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -1146,7 +1193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -1160,7 +1207,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
@@ -1174,7 +1221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
@@ -1188,7 +1235,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1">
       <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
@@ -1202,7 +1249,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1">
+    <row r="32" spans="1:5" ht="15.75" thickBot="1">
       <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
@@ -1216,33 +1263,33 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1">
+    <row r="33" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1">
       <c r="A34" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G34" s="8" t="s">
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A35" s="3" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A35" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -1262,10 +1309,13 @@
       <c r="G35" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1">
       <c r="A36" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="9">
         <v>0</v>
@@ -1286,9 +1336,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1">
+    <row r="37" spans="1:8" ht="15.75" thickBot="1">
       <c r="A37" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="4">
         <v>73</v>
@@ -1303,13 +1353,13 @@
         <v>142</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
@@ -1329,14 +1379,14 @@
         <v>149</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="6"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="41" spans="1:7" ht="16.5" thickBot="1">
+    <row r="40" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="41" spans="1:8" ht="16.5" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -1350,9 +1400,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1">
+    <row r="42" spans="1:8" ht="15.75" thickBot="1">
       <c r="A42" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="4">
         <v>3965</v>
@@ -1361,12 +1411,15 @@
         <v>5360</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A43" s="3" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A43" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="B43" s="4">
         <v>57</v>
@@ -1375,10 +1428,10 @@
         <v>73</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>8</v>
       </c>
@@ -1389,11 +1442,11 @@
         <v>73</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="46" spans="1:7" ht="16.5" thickBot="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="46" spans="1:8" ht="16.5" thickBot="1">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -1407,9 +1460,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1">
+    <row r="47" spans="1:8" ht="15.75" thickBot="1">
       <c r="A47" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" s="4">
         <v>65</v>
@@ -1420,10 +1473,13 @@
       <c r="D47" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1">
+      <c r="E47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1">
       <c r="A48" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B48" s="4">
         <v>8.1</v>
@@ -1435,9 +1491,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1">
       <c r="A49" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" s="4">
         <v>8.6999999999999993</v>
@@ -1449,9 +1505,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B50" s="4">
         <v>3.6</v>
@@ -1463,9 +1519,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1">
       <c r="A51" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B51" s="4">
         <v>27</v>
@@ -1477,9 +1533,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1">
+    <row r="52" spans="1:5" ht="15.75" thickBot="1">
       <c r="A52" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" s="4">
         <v>26</v>
@@ -1491,9 +1547,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1">
+    <row r="53" spans="1:5" ht="15.75" thickBot="1">
       <c r="A53" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="4">
         <v>25.6</v>
@@ -1505,9 +1561,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1">
+    <row r="54" spans="1:5" ht="15.75" thickBot="1">
       <c r="A54" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" s="4">
         <v>24.4</v>
@@ -1519,8 +1575,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="56" spans="1:4" ht="16.5" thickBot="1">
+    <row r="55" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="56" spans="1:5" ht="16.5" thickBot="1">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -1534,9 +1590,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1">
+    <row r="57" spans="1:5" ht="15.75" thickBot="1">
       <c r="A57" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="4">
         <v>24.3</v>
@@ -1547,10 +1603,13 @@
       <c r="D57" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E57" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" thickBot="1">
       <c r="A58" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" s="4">
         <v>144</v>
@@ -1559,12 +1618,12 @@
         <v>121</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1">
       <c r="A59" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="4">
         <v>87</v>
@@ -1576,9 +1635,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1">
+    <row r="60" spans="1:5" ht="15.75" thickBot="1">
       <c r="A60" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" s="4">
         <v>87</v>
@@ -1587,12 +1646,12 @@
         <v>48</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" thickBot="1">
       <c r="A61" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B61" s="4">
         <v>57</v>
@@ -1601,12 +1660,12 @@
         <v>73</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30.75" thickBot="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30.75" thickBot="1">
       <c r="A62" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="4">
         <v>40</v>
@@ -1618,8 +1677,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="64" spans="1:4" ht="16.5" thickBot="1">
+    <row r="63" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="64" spans="1:5" ht="16.5" thickBot="1">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -1633,9 +1692,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.75" thickBot="1">
+    <row r="65" spans="1:5" ht="15.75" thickBot="1">
       <c r="A65" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B65" s="4">
         <v>6.0000000000000001E-3</v>
@@ -1644,12 +1703,15 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A66" s="3" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A66" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
@@ -1658,11 +1720,11 @@
         <v>1</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="68" spans="1:4" ht="16.5" thickBot="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="68" spans="1:5" ht="16.5" thickBot="1">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -1676,9 +1738,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1">
+    <row r="69" spans="1:5" ht="15.75" thickBot="1">
       <c r="A69" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="4">
         <v>118</v>
@@ -1687,12 +1749,15 @@
         <v>180</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1">
+        <v>49</v>
+      </c>
+      <c r="E69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" thickBot="1">
       <c r="A70" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70" s="4">
         <v>62</v>
@@ -1701,10 +1766,10 @@
         <v>129</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" thickBot="1">
       <c r="A71" s="3" t="s">
         <v>31</v>
       </c>
@@ -1718,9 +1783,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" thickBot="1">
+    <row r="72" spans="1:5" ht="15.75" thickBot="1">
       <c r="A72" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" s="4">
         <v>2.1</v>
@@ -1732,13 +1797,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75">
+    <row r="74" spans="1:5" ht="15.75">
       <c r="A74" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="76" spans="1:4" ht="16.5" thickBot="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="76" spans="1:5" ht="16.5" thickBot="1">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -1752,9 +1817,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" thickBot="1">
+    <row r="77" spans="1:5" ht="15.75" thickBot="1">
       <c r="A77" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="4">
         <v>180</v>
@@ -1763,12 +1828,15 @@
         <v>180</v>
       </c>
       <c r="D77" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A78" s="3" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A78" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="B78" s="4">
         <v>87.84</v>
@@ -1777,11 +1845,14 @@
         <v>180</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="80" spans="1:4" ht="16.5" thickBot="1">
+        <v>76</v>
+      </c>
+      <c r="E78" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="80" spans="1:5" ht="16.5" thickBot="1">
       <c r="A80" s="12" t="s">
         <v>0</v>
       </c>
@@ -1795,9 +1866,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1">
+    <row r="81" spans="1:5" ht="15.75" thickBot="1">
       <c r="A81" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="4">
         <v>5823</v>
@@ -1806,12 +1877,15 @@
         <v>5400</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" thickBot="1">
+        <v>51</v>
+      </c>
+      <c r="E81" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1">
       <c r="A82" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="4">
         <v>2303</v>
@@ -1820,12 +1894,12 @@
         <v>2400</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="30.75" thickBot="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30.75" thickBot="1">
       <c r="A83" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="4">
         <v>3520</v>
@@ -1834,11 +1908,11 @@
         <v>3000</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="85" spans="1:4" ht="16.5" thickBot="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="85" spans="1:5" ht="16.5" thickBot="1">
       <c r="A85" s="12" t="s">
         <v>0</v>
       </c>
@@ -1852,9 +1926,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="30.75" thickBot="1">
+    <row r="86" spans="1:5" ht="30.75" thickBot="1">
       <c r="A86" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B86" s="4">
         <v>50.1</v>
@@ -1863,12 +1937,15 @@
         <v>43.2</v>
       </c>
       <c r="D86" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E86" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A87" s="3" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A87" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="B87" s="4">
         <v>21.1</v>
@@ -1877,12 +1954,12 @@
         <v>15</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" thickBot="1">
       <c r="A88" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B88" s="4">
         <v>3.5</v>
@@ -1891,12 +1968,12 @@
         <v>3</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" thickBot="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" thickBot="1">
       <c r="A89" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B89" s="4">
         <v>17.5</v>
@@ -1905,12 +1982,12 @@
         <v>12</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15.75" thickBot="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" thickBot="1">
       <c r="A90" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B90" s="4">
         <v>0.1</v>
@@ -1919,12 +1996,12 @@
         <v>0</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15.75" thickBot="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" thickBot="1">
       <c r="A91" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" s="4">
         <v>0</v>
@@ -1933,12 +2010,12 @@
         <v>0</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" thickBot="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" thickBot="1">
       <c r="A92" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B92" s="4">
         <v>29</v>
@@ -1947,11 +2024,11 @@
         <v>28.2</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="94" spans="1:4" ht="16.5" thickBot="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="94" spans="1:5" ht="16.5" thickBot="1">
       <c r="A94" s="12" t="s">
         <v>0</v>
       </c>
@@ -1965,9 +2042,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="30.75" thickBot="1">
+    <row r="95" spans="1:5" ht="30.75" thickBot="1">
       <c r="A95" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B95" s="4">
         <v>26</v>
@@ -1978,10 +2055,13 @@
       <c r="D95" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E95" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" thickBot="1">
       <c r="A96" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B96" s="4">
         <v>26</v>
@@ -1995,7 +2075,7 @@
     </row>
     <row r="97" spans="1:4" ht="15.75" thickBot="1">
       <c r="A97" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B97" s="4">
         <v>0</v>
@@ -2004,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>